<commit_message>
modified code to add more scenarios and locators
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>test step</t>
   </si>
@@ -48,15 +48,9 @@
     <t>enter email address</t>
   </si>
   <si>
-    <t>naveenanimation20@gmail.com</t>
-  </si>
-  <si>
     <t>enter password</t>
   </si>
   <si>
-    <t>Test@1234</t>
-  </si>
-  <si>
     <t>click on login button</t>
   </si>
   <si>
@@ -97,6 +91,42 @@
   </si>
   <si>
     <t>loginBtn</t>
+  </si>
+  <si>
+    <t>verify home page header</t>
+  </si>
+  <si>
+    <t>get home page header text</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//h1[text()='Sales Dashboard']</t>
+  </si>
+  <si>
+    <t>isDisplayed</t>
+  </si>
+  <si>
+    <t>anubhat20@yahoo.co.in</t>
+  </si>
+  <si>
+    <t>Testing@1234</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>dashboard-selector__title</t>
+  </si>
+  <si>
+    <t>getText</t>
+  </si>
+  <si>
+    <t>Sales Dashboard</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -149,10 +179,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,16 +479,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -467,10 +499,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -518,47 +550,47 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -566,41 +598,41 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -609,43 +641,9 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -653,20 +651,119 @@
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>